<commit_message>
Samsumng specs scraping and writing done
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/OvenTemplate.xlsx
+++ b/Scrape_Bot1/Data/OvenTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04AC49-8CBD-45A8-AF49-BA0BA0DBB4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0EC1A5-C6A2-48D2-B1C6-3885F0EB5A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Brand</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Capacity (in liters)</t>
-  </si>
-  <si>
-    <t>Heating Method</t>
   </si>
   <si>
     <t>Color</t>
@@ -462,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,18 +473,17 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,11 +538,8 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amazon bot 4 ultra done
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/OvenTemplate.xlsx
+++ b/Scrape_Bot1/Data/OvenTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F894A217-89A5-417E-AEA8-C41283127B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA86C9F3-0222-4BAF-A6D8-4D650B1EBBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Brand</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>New product</t>
+  </si>
+  <si>
+    <t>Amazon Offer Price</t>
+  </si>
+  <si>
+    <t>Amazon URL</t>
+  </si>
+  <si>
+    <t>Amazon MRP</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,20 +483,22 @@
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="65.44140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,45 +518,54 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bot 4 ultra flipkart done
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/OvenTemplate.xlsx
+++ b/Scrape_Bot1/Data/OvenTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA86C9F3-0222-4BAF-A6D8-4D650B1EBBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F54F281-88A7-41B0-BF88-31ED8E7A9EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Brand</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Amazon MRP</t>
+  </si>
+  <si>
+    <t>Flipkart URL</t>
+  </si>
+  <si>
+    <t>Flipkart Offer Price</t>
+  </si>
+  <si>
+    <t>Flipkart MRP</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,20 +494,20 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="7" width="12.77734375" customWidth="1"/>
     <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,45 +536,54 @@
         <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>